<commit_message>
methodes updated and the project updated
</commit_message>
<xml_diff>
--- a/methodes necessaires/methodes.xlsx
+++ b/methodes necessaires/methodes.xlsx
@@ -15,8 +15,249 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Xue CAO</author>
+  </authors>
+  <commentList>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Favoris&gt; liste = FavorisManager.getListeFavorisOnline(1);
+  for(Favoris f : liste){
+   System.out.println(f);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Photo&gt; liste = PhotoManager.getPhotosByMemberId(1);
+  for(Photo p : liste){
+   System.out.println(p);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Photo&gt; liste = PhotoManager.getProfilPhotosByMemberId(1);
+  for(Photo p : liste){
+   System.out.println(p);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ArrayList&lt;Favoris&gt; liste = FavorisManager.getFavorisByMemberId(1);</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Photo&gt; liste = PhotoManager.getProfilPhotosByMemberId(1);
+  for(Photo p : liste){
+   System.out.println(p);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FavorisManager.deleteFavoris(23, 30)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Clinsdoeil clin = new Clinsdoeil();
+  clin.setFromId(1);
+  clin.setToId(2);;
+ClinsdoeilManager.addClindoeil(clin);</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FavorisManager.addFavoris(new Date(), 23, 30)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+MessageManager.marquerMessages(2, false);</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Profile.xhtml:</t>
   </si>
@@ -33,15 +274,9 @@
     <t xml:space="preserve">3- get photo profile user par id du user = </t>
   </si>
   <si>
-    <t>PhotoManager.getProfilPhoto(membre.getMembreId());</t>
-  </si>
-  <si>
     <t xml:space="preserve">4- liste de messages recus du user par id du user = </t>
   </si>
   <si>
-    <t>MessageManager.getListeMessagesRecus(membre.getMembreId());</t>
-  </si>
-  <si>
     <t xml:space="preserve">6- liste des favoris =  </t>
   </si>
   <si>
@@ -96,9 +331,6 @@
     <t>27- StatusManager.getStatusById(status_id);</t>
   </si>
   <si>
-    <t xml:space="preserve"> MessageManager.getListeMessagesEnvoyes(membre.getMembreId());</t>
-  </si>
-  <si>
     <t>5- liste de messages envoyes par le user par id du user</t>
   </si>
   <si>
@@ -159,26 +391,68 @@
     <t>MembreManager.supprimerMembre(Membre m)</t>
   </si>
   <si>
-    <t>ClinDoeilManager.insertClinDoeil(Membre m, Membre m) OU (user id, user id)</t>
-  </si>
-  <si>
     <t>28 - Marquer toutes les messages comme lues</t>
   </si>
   <si>
-    <t>MessageManager.marquerMessagesCommeLues();</t>
-  </si>
-  <si>
     <t>29- recherche dynamique avec hashtmap</t>
   </si>
   <si>
     <t>MembreManager.recherche(Hashmap criteresRecherche);</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Favoris&gt; getFavorisByMemberId(int membreFavorisantId)</t>
+  </si>
+  <si>
+    <t>public static int addFavoris(Date date, int membreFavorisantId, int membreFavoriseId)</t>
+  </si>
+  <si>
+    <t>public static int deleteFavoris(int membreFavorisantId, int membreFavoriseId)</t>
+  </si>
+  <si>
+    <t>public static int addClindoeil(Clinsdoeil clin)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Photo&gt; getPhotosByMemberId(int memberID)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Photo&gt; getProfilPhotosByMemberId(int memberID)</t>
+  </si>
+  <si>
+    <t>public static int addPhoto(Photo photo)</t>
+  </si>
+  <si>
+    <t>public static int deletePhoto(int photoId)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Message&gt; getListeMessagesEnvoyesByMemberId(int memberId)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Message&gt; getListeMessagesRecusByMemberId(int memberId)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Message&gt; getListeMessagesByMembers(int fromId,int toId)</t>
+  </si>
+  <si>
+    <t>public static int addMessage(Message m)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Clinsdoeil&gt; getClinsdoeilRecus(int fromId)</t>
+  </si>
+  <si>
+    <t>public static int getNombreClinRecus(int membreId)</t>
+  </si>
+  <si>
+    <t>public static int marquerMessages(int toId,Boolean dejaLu)</t>
+  </si>
+  <si>
+    <t>j'ai besoin tous les criteres de recherche</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,13 +460,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -207,8 +521,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,244 +821,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
-    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.5703125" customWidth="1"/>
+    <col min="2" max="2" width="79" customWidth="1"/>
+    <col min="3" max="3" width="78.85546875" customWidth="1"/>
+    <col min="4" max="4" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" s="3"/>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="B27" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="B29" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+      <c r="C29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
         <v>15</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" t="s">
-        <v>49</v>
+      <c r="B44" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update liste methodes - 15/07 10:25
</commit_message>
<xml_diff>
--- a/methodes necessaires/methodes.xlsx
+++ b/methodes necessaires/methodes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
   <si>
     <t>Profile.xhtml:</t>
   </si>
@@ -238,16 +238,65 @@
   </si>
   <si>
     <t>Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NiveauMembreManager.getNiveauById(niveauMembre);</t>
+  </si>
+  <si>
+    <t>Return = Objet NiveauMembre</t>
+  </si>
+  <si>
+    <t>return= objet categorie</t>
+  </si>
+  <si>
+    <t>return= objet hair color</t>
+  </si>
+  <si>
+    <t>return= objet skin color</t>
+  </si>
+  <si>
+    <t>return= objet eye color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">return= objet weightRange </t>
+  </si>
+  <si>
+    <t>return= objet city</t>
+  </si>
+  <si>
+    <t>return= objetStatus</t>
+  </si>
+  <si>
+    <t>HobbyManager.getHobbyById(Integer);</t>
+  </si>
+  <si>
+    <t>return = objet hobby</t>
+  </si>
+  <si>
+    <t>MembreManager.setUserOnline(id User);</t>
+  </si>
+  <si>
+    <t>return int</t>
+  </si>
+  <si>
+    <t>MembreManager.setUserOffline(id User);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -279,12 +328,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,13 +631,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.85546875" customWidth="1"/>
     <col min="2" max="2" width="100.42578125" customWidth="1"/>
     <col min="3" max="3" width="54.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
@@ -767,45 +817,74 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B36" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B37" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B38" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B39" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B40" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B41" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="B42" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -813,129 +892,147 @@
       <c r="A45" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="1">
+      <c r="A48" s="3">
         <v>32</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="1">
+      <c r="A49" s="3">
         <v>33</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="1">
+      <c r="A50" s="3">
         <v>34</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="1">
+      <c r="A51" s="3">
         <v>35</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="C52" s="2" t="s">
+      <c r="A52" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="C53" s="2" t="s">
+      <c r="A53" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="C54" s="2" t="s">
+      <c r="A54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="1" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Imagepath dans le bean membre
</commit_message>
<xml_diff>
--- a/methodes necessaires/methodes.xlsx
+++ b/methodes necessaires/methodes.xlsx
@@ -15,8 +15,566 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Xue CAO</author>
+  </authors>
+  <commentList>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Favoris&gt; liste = FavorisManager.getListeFavorisOnline(1);
+  for(Favoris f : liste){
+   System.out.println(f);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Photo&gt; liste = PhotoManager.getPhotosByMemberId(1);
+  for(Photo p : liste){
+   System.out.println(p);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Photo&gt; liste = PhotoManager.getProfilPhotosByMemberId(1);
+  for(Photo p : liste){
+   System.out.println(p);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ArrayList&lt;Favoris&gt; liste = FavorisManager.getFavorisByMemberId(1);</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ArrayList&lt;Favoris&gt; liste = FavorisManager.getFavorisByMemberId(1);</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Photo&gt; liste = PhotoManager.getProfilPhotosByMemberId(1);
+  for(Photo p : liste){
+   System.out.println(p);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Categorie&gt; list = CategorieManager.getListeCategories();
+  for(Categorie c : list){
+   System.out.println(c);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;HairColor&gt; list = HairColorManager.getListeHairColors();
+  for(HairColor c : list){
+   System.out.println(c);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;SkinColor&gt; list = SkinColorManager.getListeSkinColors();
+  for(SkinColor c : list){
+   System.out.println(c);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;EyeColor&gt; list = EyeColorManager.getListeEyeColors();
+  for(EyeColor c : list){
+   System.out.println(c);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;HeightRange&gt; list = HeightRangeManager.getListeHeightRanges();
+  for(HeightRange c : list){
+   System.out.println(c);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;WeightRange&gt; list = WeightRangeManager.getListeWeightRanges();
+  for(WeightRange c : list){
+   System.out.println(c);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;City&gt; list = CityManager.getListeCities();
+  for(City c : list){
+   System.out.println(c);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Hobby&gt; list = HobbyManager.getListeHobbies();
+  for(Hobby c : list){
+   System.out.println(c);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  ArrayList&lt;Status&gt; list = StatusManager.getListeStatus();
+  for(Status c : list){
+   System.out.println(c);
+  }</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FavorisManager.deleteFavoris(23, 30)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Clinsdoeil clin = new Clinsdoeil();
+  clin.setFromId(1);
+  clin.setToId(2);;
+ClinsdoeilManager.addClindoeil(clin);</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FavorisManager.addFavoris(new Date(), 23, 30)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  Categorie c = CategorieManager.getCategorieById(1);
+   System.out.println(c);</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+  HairColor c = HairColorManager.getListeHairColorById(1);
+   System.out.println(c);</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xue CAO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+MessageManager.marquerMessages(2, false);</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="128">
   <si>
     <t>Profile.xhtml:</t>
   </si>
@@ -276,17 +834,137 @@
     <t>MembreManager.setUserOnline(id User);</t>
   </si>
   <si>
-    <t>return int</t>
-  </si>
-  <si>
     <t>MembreManager.setUserOffline(id User);</t>
+  </si>
+  <si>
+    <t>return int  Requete type Update</t>
+  </si>
+  <si>
+    <t>ClinsdoeilManager.getNombreClinRecus(membre.getMembreId());</t>
+  </si>
+  <si>
+    <t>return = int requete select count</t>
+  </si>
+  <si>
+    <t>public static int deletePhoto(int photoId)</t>
+  </si>
+  <si>
+    <t>public static int addPhoto(Photo photo)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Photo&gt; getProfilPhotosByMemberId(int memberID)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Photo&gt; getPhotosByMemberId(int memberID)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Message&gt; getListeMessagesRecusByMemberId(int memberId)</t>
+  </si>
+  <si>
+    <t>public static int addMessage(Message m)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Message&gt; getListeMessagesEnvoyesByMemberId(int memberId)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Message&gt; getListeMessagesByMembers(int fromId,int toId)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Favoris&gt; getFavorisByMemberId(int membreFavorisantId)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Clinsdoeil&gt; getClinsdoeilRecus(int fromId)</t>
+  </si>
+  <si>
+    <t>public static int getNombreClinRecus(int membreId)</t>
+  </si>
+  <si>
+    <t>public static int addClindoeil(Clinsdoeil clin)</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Categorie&gt; getListeCategories()</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;HairColor&gt; getListeHairColors()</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;SkinColor&gt; getListeSkinColors()</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;EyeColor&gt; getListeEyeColors()</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;HeightRange&gt; getListeHeightRanges()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> public static ArrayList&lt;WeightRange&gt; getListeWeightRanges()</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;City&gt; getListeCities()</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Hobby&gt; getListeHobbies()</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Status&gt; getListeStatus()</t>
+  </si>
+  <si>
+    <t>public static int deleteFavoris(int membreFavorisantId, int membreFavoriseId)</t>
+  </si>
+  <si>
+    <t>public static int addFavoris(Date date, int membreFavorisantId, int membreFavoriseId)</t>
+  </si>
+  <si>
+    <t>21- CategorieManager.getCategorieById(categorie);</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> public static Categorie getCategorieById(int id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> public static HairColor  getListeHairColorById(int id)</t>
+  </si>
+  <si>
+    <t>public static SkinColor getListeSkinColorById(int id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> public static EyeColor getListeEyeColorById(int id)</t>
+  </si>
+  <si>
+    <t>public static WeightRange getWeightRangeById(int id)</t>
+  </si>
+  <si>
+    <t>public static City getCityById(int i)</t>
+  </si>
+  <si>
+    <t>public static Status getStatusById(int i)</t>
+  </si>
+  <si>
+    <t>public static int marquerMessages(int toId,Boolean dejaLu)</t>
+  </si>
+  <si>
+    <t>MembreManager.recherche(Hashmap criteresRecherche);</t>
+  </si>
+  <si>
+    <t>j'ai besoin tous les criteres de recherche</t>
+  </si>
+  <si>
+    <t>HobbyManager.getListeHobbiesUser(userID);</t>
+  </si>
+  <si>
+    <t>return= arraylist hobby</t>
+  </si>
+  <si>
+    <t>public static ArrayList&lt;Hobby&gt; getListeHobbiesByMembreId(int id)</t>
+  </si>
+  <si>
+    <t>AJOUTER un attribut String IMAGEPATH dans le bean membre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,8 +979,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,6 +1017,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,13 +1045,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,10 +1351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1005,7 +1727,7 @@
         <v>85</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>58</v>
@@ -1016,10 +1738,10 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>59</v>
@@ -1029,11 +1751,30 @@
       </c>
     </row>
     <row r="55" spans="1:4">
+      <c r="A55" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="C55" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1044,13 +1785,329 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="B44" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update methodes- 16/07 11:24
</commit_message>
<xml_diff>
--- a/methodes necessaires/methodes.xlsx
+++ b/methodes necessaires/methodes.xlsx
@@ -574,7 +574,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="140">
   <si>
     <t>Profile.xhtml:</t>
   </si>
@@ -960,7 +960,40 @@
     <t>AJOUTER un attribut String IMAGEPATH dans le bean membre</t>
   </si>
   <si>
-    <t>MembreManager.ajouterFavoris(mbb.getMembre(), membre);</t>
+    <t>inner join avec MEMBRE pour recuperer l'image du profile du MEMBRE qui a envoye  le message</t>
+  </si>
+  <si>
+    <t>AJOUTER un attribut String IMAGEPATH dans le bean MESSAGE</t>
+  </si>
+  <si>
+    <t>AJOUTER un attribut String PSEUDO dans le bean MESSAGE</t>
+  </si>
+  <si>
+    <t>inner join avec MEMBRE pour recuperer le Pseudo du profile du MEMBRE qui a envoye  le message</t>
+  </si>
+  <si>
+    <t>AJOUTER un attribut String IMAGEPATH dans le bean CLINSDOEIL</t>
+  </si>
+  <si>
+    <t>AJOUTER un attribut String PSEUDO dans le bean  CLINSDOEIL</t>
+  </si>
+  <si>
+    <t>inner join avec MEMBRE pour recuperer l'image du profile du MEMBRE qui a envoye  le  CLINSDOEIL</t>
+  </si>
+  <si>
+    <t>inner join avec MEMBRE pour recuperer le Pseudo du profile du MEMBRE qui a envoye  le CLINSDOEIL</t>
+  </si>
+  <si>
+    <t>get toute la liste de niveux de membre</t>
+  </si>
+  <si>
+    <t>return= objet niveaumembre</t>
+  </si>
+  <si>
+    <t>get membre by id</t>
+  </si>
+  <si>
+    <t>MembreManager.getMembreById(int memberid)</t>
   </si>
 </sst>
 </file>
@@ -1354,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1782,8 +1815,55 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B60" t="s">
         <v>128</v>
       </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B61" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1795,7 +1875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajout de methodes et update backings
</commit_message>
<xml_diff>
--- a/methodes necessaires/methodes.xlsx
+++ b/methodes necessaires/methodes.xlsx
@@ -574,7 +574,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="146">
   <si>
     <t>Profile.xhtml:</t>
   </si>
@@ -994,6 +994,24 @@
   </si>
   <si>
     <t>MembreManager.getMembreById(int memberid)</t>
+  </si>
+  <si>
+    <t>get membre by nickname(nickname)</t>
+  </si>
+  <si>
+    <t>get membre by nickname et password(nickname+password)</t>
+  </si>
+  <si>
+    <t>MessageManager.deleteMessage(Message message);</t>
+  </si>
+  <si>
+    <t>getClinsdoeilRecus(int TOId){</t>
+  </si>
+  <si>
+    <t>arraylist clinsdoeils qui un user a recu!</t>
+  </si>
+  <si>
+    <t>ClinsdoeilManager.deleteClindoeil(Clinsdoeil clin){</t>
   </si>
 </sst>
 </file>
@@ -1387,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:B67"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1862,8 +1880,33 @@
       </c>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="2"/>
+      <c r="A68" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>145</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1875,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>